<commit_message>
added date and time
</commit_message>
<xml_diff>
--- a/examples/prueba.xlsx
+++ b/examples/prueba.xlsx
@@ -27,6 +27,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="mmm d yyyy hh:mm AM/PM"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -64,9 +67,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -416,7 +420,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -445,6 +449,11 @@
         <v>123.456</v>
       </c>
     </row>
+    <row r="5" spans="1:1">
+      <c r="A5" s="2">
+        <v>42824.37045138889</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>